<commit_message>
Finished drafting test script; compiled data files out of R
</commit_message>
<xml_diff>
--- a/dummy1.xlsx
+++ b/dummy1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherineeisen/github/oenothera/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FABA341-36F1-654B-A5CB-516FEE00099D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C0EFF1-8A00-4D4C-AE4A-A3270BE509F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23560" yWindow="7300" windowWidth="27640" windowHeight="16940" xr2:uid="{5F5D0AD8-8A61-874A-B263-7418653EE2EC}"/>
+    <workbookView xWindow="33040" yWindow="8800" windowWidth="27640" windowHeight="16940" xr2:uid="{5F5D0AD8-8A61-874A-B263-7418653EE2EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,133 +27,133 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
-    <t>rm3-1</t>
-  </si>
-  <si>
-    <t>rm3-2</t>
-  </si>
-  <si>
-    <t>rm3-4-1</t>
-  </si>
-  <si>
-    <t>rm3-7</t>
-  </si>
-  <si>
-    <t>rm3-8</t>
-  </si>
-  <si>
-    <t>2methylbutyronitrile</t>
-  </si>
-  <si>
-    <t>3methylbutyronitrile</t>
-  </si>
-  <si>
-    <t>b-myrcene</t>
-  </si>
-  <si>
-    <t>cis-b-ocimene</t>
-  </si>
-  <si>
-    <t>trans-b-ocimene</t>
-  </si>
-  <si>
-    <t>nitro-2-methyl butane</t>
-  </si>
-  <si>
-    <t>nitro-3-methyl butane</t>
-  </si>
-  <si>
-    <t>pyran lin oxide ketone</t>
-  </si>
-  <si>
-    <t>linalool</t>
-  </si>
-  <si>
-    <t>beta-caryophyllene</t>
-  </si>
-  <si>
-    <t>beta farnesene</t>
-  </si>
-  <si>
-    <t>alpha humulene</t>
-  </si>
-  <si>
-    <t>alpha terpineol</t>
-  </si>
-  <si>
-    <t>Z,E alpha farnesene</t>
-  </si>
-  <si>
-    <t>E,E alpha farnesene</t>
-  </si>
-  <si>
-    <t>nerol?</t>
-  </si>
-  <si>
-    <t>geraniol</t>
-  </si>
-  <si>
-    <t>2phenylethanol</t>
-  </si>
-  <si>
-    <t>phenylacetonitrile</t>
-  </si>
-  <si>
-    <t>caryophyllene oxide</t>
-  </si>
-  <si>
-    <t>nerolidol</t>
-  </si>
-  <si>
-    <t>nitrophenylethane</t>
-  </si>
-  <si>
-    <t>phenylacetaldoxime</t>
-  </si>
-  <si>
-    <t>isophytol</t>
-  </si>
-  <si>
-    <t>farnesol</t>
-  </si>
-  <si>
-    <t>farnesene epoxide 1</t>
-  </si>
-  <si>
-    <t>farnesene epoxide 2</t>
-  </si>
-  <si>
     <t>Compound</t>
   </si>
   <si>
-    <t>furanoid lin oxide 1</t>
-  </si>
-  <si>
-    <t>furanoid lin oxide 2</t>
-  </si>
-  <si>
-    <t>isobutyronitrile 1</t>
-  </si>
-  <si>
-    <t>isobutyronitrile 2</t>
-  </si>
-  <si>
-    <t>2-methylbutyraldoxime 1</t>
-  </si>
-  <si>
-    <t>3-methylbutyraldoxime 1</t>
-  </si>
-  <si>
-    <t>2-methylbutyraldoxime 2</t>
-  </si>
-  <si>
-    <t>3-methylbutyraldoxime 2</t>
-  </si>
-  <si>
-    <t>pyranoid linalool oxide 1</t>
-  </si>
-  <si>
-    <t>pyranoid linalool oxide 2</t>
+    <t>Comp.2methylbutyronitrile</t>
+  </si>
+  <si>
+    <t>Comp.3methylbutyronitrile</t>
+  </si>
+  <si>
+    <t>Comp.b-myrcene</t>
+  </si>
+  <si>
+    <t>Comp.cis-b-ocimene</t>
+  </si>
+  <si>
+    <t>Comp.trans-b-ocimene</t>
+  </si>
+  <si>
+    <t>Comp.nitro-2-methyl-butane</t>
+  </si>
+  <si>
+    <t>Comp.nitro-3-methyl-butane</t>
+  </si>
+  <si>
+    <t>Comp.isobutyronitrile1</t>
+  </si>
+  <si>
+    <t>Comp.isobutyronitrile2</t>
+  </si>
+  <si>
+    <t>Comp.furanoid-lin-oxide1</t>
+  </si>
+  <si>
+    <t>Comp.furanoid-lin-oxide2</t>
+  </si>
+  <si>
+    <t>Comp.pyran-lin-oxide-ketone</t>
+  </si>
+  <si>
+    <t>Comp.2-methylbutyraldoxime1</t>
+  </si>
+  <si>
+    <t>Comp.3-methylbutyraldoxime1</t>
+  </si>
+  <si>
+    <t>Comp.2-methylbutyraldoxime2</t>
+  </si>
+  <si>
+    <t>Comp.3-methylbutyraldoxime2</t>
+  </si>
+  <si>
+    <t>Comp.linalool</t>
+  </si>
+  <si>
+    <t>Comp.beta-caryophyllene</t>
+  </si>
+  <si>
+    <t>Comp.beta-farnesene</t>
+  </si>
+  <si>
+    <t>Comp.alpha-humulene</t>
+  </si>
+  <si>
+    <t>Comp.alpha-terpineol</t>
+  </si>
+  <si>
+    <t>Comp.Z-E-alpha-farnesene</t>
+  </si>
+  <si>
+    <t>Comp.pyranoid-linalool-oxide1</t>
+  </si>
+  <si>
+    <t>Comp.E-E-alpha-farnesene</t>
+  </si>
+  <si>
+    <t>Comp.pyranoid-linalool-oxide2</t>
+  </si>
+  <si>
+    <t>Comp.nerol</t>
+  </si>
+  <si>
+    <t>Comp.geraniol</t>
+  </si>
+  <si>
+    <t>Comp.2phenylethanol</t>
+  </si>
+  <si>
+    <t>Comp.phenylacetonitrile</t>
+  </si>
+  <si>
+    <t>Comp.farnesene epoxide1</t>
+  </si>
+  <si>
+    <t>Comp.caryophyllene-oxide</t>
+  </si>
+  <si>
+    <t>Comp.nerolidol</t>
+  </si>
+  <si>
+    <t>Comp.farnesene-epoxide2</t>
+  </si>
+  <si>
+    <t>Comp.nitrophenylethane</t>
+  </si>
+  <si>
+    <t>Comp.phenylacetaldoxime</t>
+  </si>
+  <si>
+    <t>Comp.isophytol</t>
+  </si>
+  <si>
+    <t>Comp.farnesol</t>
+  </si>
+  <si>
+    <t>Samp.rm3-1</t>
+  </si>
+  <si>
+    <t>Samp.rm3-2</t>
+  </si>
+  <si>
+    <t>Samp.rm3-4-1</t>
+  </si>
+  <si>
+    <t>Samp.rm3-7</t>
+  </si>
+  <si>
+    <t>Samp.rm3-8</t>
   </si>
 </sst>
 </file>
@@ -526,47 +526,47 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>125437</v>
@@ -586,7 +586,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>42624</v>
@@ -600,7 +600,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>3396543</v>
@@ -614,7 +614,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>47061</v>
@@ -622,22 +622,22 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="C11">
         <v>11778</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <v>36936</v>
@@ -670,7 +670,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="B14">
         <v>1687312</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="B15">
         <v>121417</v>
@@ -710,7 +710,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="B16">
         <v>392505</v>
@@ -730,7 +730,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>40167</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18">
         <v>4137927</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B19">
         <v>139658</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B20">
         <v>98570</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D21">
         <v>97321</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B22">
         <v>58652</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B23">
         <v>77526</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1"/>
       <c r="F24">
@@ -843,7 +843,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B25">
         <v>47081057</v>
@@ -852,7 +852,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1"/>
       <c r="D26">
@@ -864,12 +864,12 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28">
@@ -882,7 +882,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>213375</v>
@@ -894,7 +894,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>96549</v>
@@ -905,7 +905,7 @@
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="C31" s="2"/>
@@ -915,7 +915,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B32" s="1"/>
       <c r="D32">
@@ -928,7 +928,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B33">
         <v>75502</v>
@@ -936,8 +936,8 @@
       <c r="F33" s="1"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>31</v>
+      <c r="A34" t="s">
+        <v>33</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="2"/>
@@ -946,8 +946,8 @@
       <c r="F34" s="1"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>26</v>
+      <c r="A35" t="s">
+        <v>34</v>
       </c>
       <c r="B35">
         <v>160200</v>
@@ -958,8 +958,8 @@
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>27</v>
+      <c r="A36" t="s">
+        <v>35</v>
       </c>
       <c r="B36">
         <v>683773</v>
@@ -967,7 +967,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B37">
         <v>182147</v>
@@ -984,7 +984,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38">

</xml_diff>